<commit_message>
Planilha de riscos atualizada
</commit_message>
<xml_diff>
--- a/Sprint2/Documentação/Planilha de Risco Excel.xlsx
+++ b/Sprint2/Documentação/Planilha de Risco Excel.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\look\Documents\Senssky\Sprint2\Documentação\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAE3855-2FFD-46DE-9AA3-20581772F1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2C02C10-118D-4A9B-A6B9-459F1F12E9AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>Riscos</t>
   </si>
@@ -103,13 +97,7 @@
     <t>MÉDIA/ALTA</t>
   </si>
   <si>
-    <t>GRAVE</t>
-  </si>
-  <si>
     <t>MÉDIO</t>
-  </si>
-  <si>
-    <t>GRAVÍSSIMO</t>
   </si>
   <si>
     <t>Levar mais de um
@@ -148,12 +136,39 @@
 aconteça, alguem consiga
 te levar</t>
   </si>
+  <si>
+    <t>ALTA</t>
+  </si>
+  <si>
+    <t>IMPACTO</t>
+  </si>
+  <si>
+    <t>PROBABILIDADE</t>
+  </si>
+  <si>
+    <t>AÇÃO</t>
+  </si>
+  <si>
+    <t>MITIGAR</t>
+  </si>
+  <si>
+    <t>EVITAR</t>
+  </si>
+  <si>
+    <t>ALTA 3</t>
+  </si>
+  <si>
+    <t>MÉDIA 2</t>
+  </si>
+  <si>
+    <t>BAIXA 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,8 +189,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.39997558519241921"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,12 +206,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -202,18 +218,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -226,24 +230,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD36B6B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEAE890"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA565D9"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -251,40 +285,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -355,7 +475,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -407,7 +527,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -621,29 +741,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227551E8-D6F7-4628-A739-FBF455FCCFC6}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="49.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.875" customWidth="1"/>
+    <col min="2" max="2" width="19.375" customWidth="1"/>
+    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="54" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="13" max="13" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,107 +776,211 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="57">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="57" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="D2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+    </row>
+    <row r="3" spans="1:13" ht="57">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="19">
+        <v>3</v>
+      </c>
+      <c r="K3" s="20">
+        <v>6</v>
+      </c>
+      <c r="L3" s="29">
+        <v>9</v>
+      </c>
+      <c r="M3" s="25"/>
+    </row>
+    <row r="4" spans="1:13" ht="57">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="28">
+        <v>2</v>
+      </c>
+      <c r="K4" s="26">
+        <v>4</v>
+      </c>
+      <c r="L4" s="27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="57">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="D5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="21">
+        <v>1</v>
+      </c>
+      <c r="K5" s="22">
+        <v>2</v>
+      </c>
+      <c r="L5" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="71.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="C6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="85.5">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="57" x14ac:dyDescent="0.25">
+      <c r="D7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="24"/>
+    </row>
+    <row r="8" spans="1:13" ht="57">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="C8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7">
+      <c r="E25" s="10"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="5:7">
+      <c r="E26" s="11"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="5:7">
+      <c r="E27" s="12"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>